<commit_message>
[ADD] product_upload - agregamos el parent product
</commit_message>
<xml_diff>
--- a/product_upload/tests/products_0.xlsx
+++ b/product_upload/tests/products_0.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t xml:space="preserve">Referencia</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">Código mercadolibre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
   </si>
   <si>
     <t xml:space="preserve">D25811K-AR-DECKER</t>
@@ -174,19 +177,22 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -217,14 +223,16 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>9490.76</v>
@@ -233,7 +241,7 @@
         <v>10000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.155</v>
@@ -245,7 +253,7 @@
         <v>885911484848</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -268,21 +276,24 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,14 +324,16 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>9490.76</v>
@@ -329,13 +342,16 @@
         <v>10000</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.21</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>0.21</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>4502015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] product_upload -  test
</commit_message>
<xml_diff>
--- a/product_upload/tests/products_0.xlsx
+++ b/product_upload/tests/products_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="B&amp;D" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t xml:space="preserve">Referencia</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">Accesorio - Discos para TE-XC 110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3423</t>
   </si>
 </sst>
 </file>
@@ -182,17 +185,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,24 +279,24 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -350,8 +353,8 @@
       <c r="G2" s="2" t="n">
         <v>0.21</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>4502015</v>
+      <c r="J2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] product_upload - agregar columna vendors - mejorar los tests - reforzar el manjo de errores al procesar la planilla
</commit_message>
<xml_diff>
--- a/product_upload/tests/products_0.xlsx
+++ b/product_upload/tests/products_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="B&amp;D" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t xml:space="preserve">Referencia</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve">17 MM HEX DEDICATED CHIPPING HAMMER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">885911484848</t>
   </si>
   <si>
     <t xml:space="preserve">MELICODE123</t>
@@ -179,23 +182,23 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,11 +255,11 @@
       <c r="G2" s="2" t="n">
         <v>0.155</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>885911484848</v>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -278,25 +281,25 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,7 +336,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -345,7 +348,7 @@
         <v>10000</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.21</v>
@@ -354,7 +357,7 @@
         <v>0.21</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] corregir y mejorar test
</commit_message>
<xml_diff>
--- a/product_upload/tests/products_0.xlsx
+++ b/product_upload/tests/products_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="B&amp;D" sheetId="1" state="visible" r:id="rId2"/>
@@ -182,23 +182,23 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,25 +281,25 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>